<commit_message>
Finalize list of aircrafts
</commit_message>
<xml_diff>
--- a/AIRCRAFTS.xlsx
+++ b/AIRCRAFTS.xlsx
@@ -3106,7 +3106,9 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
@@ -3118,7 +3120,9 @@
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
@@ -3130,7 +3134,9 @@
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>140</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
@@ -3142,7 +3148,9 @@
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>165</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
@@ -3154,7 +3162,9 @@
       <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <v>185</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
@@ -3166,7 +3176,9 @@
       <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
@@ -3178,7 +3190,9 @@
       <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>266</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
@@ -3190,7 +3204,9 @@
       <c r="C11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
@@ -3202,7 +3218,9 @@
       <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <v>228</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
@@ -3214,7 +3232,9 @@
       <c r="C13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2">
+        <v>187</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
@@ -3226,7 +3246,9 @@
       <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>240</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
@@ -3238,7 +3260,9 @@
       <c r="C15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2">
+        <v>107</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
@@ -3250,7 +3274,9 @@
       <c r="C16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>140</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
@@ -3262,7 +3288,9 @@
       <c r="C17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2">
+        <v>140</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
@@ -3274,7 +3302,9 @@
       <c r="C18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2">
+        <v>140</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
@@ -3286,7 +3316,9 @@
       <c r="C19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2">
+        <v>165</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
@@ -3298,7 +3330,9 @@
       <c r="C20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <v>165</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
@@ -3310,7 +3344,9 @@
       <c r="C21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2">
+        <v>185</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1" t="s">
@@ -3322,7 +3358,9 @@
       <c r="C22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2">
+        <v>185</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1" t="s">
@@ -3334,7 +3372,9 @@
       <c r="C23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2">
+        <v>259</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1" t="s">
@@ -3346,7 +3386,9 @@
       <c r="C24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>440</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1" t="s">
@@ -3358,7 +3400,9 @@
       <c r="C25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1" t="s">
@@ -3370,7 +3414,9 @@
       <c r="C26" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1" t="s">
@@ -3382,7 +3428,9 @@
       <c r="C27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1" t="s">
@@ -3394,7 +3442,9 @@
       <c r="C28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2">
+        <v>260</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1" t="s">
@@ -3406,7 +3456,9 @@
       <c r="C29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2">
+        <v>300</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1" t="s">
@@ -3418,7 +3470,9 @@
       <c r="C30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2">
+        <v>261</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1" t="s">
@@ -3430,7 +3484,9 @@
       <c r="C31" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>295</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1" t="s">
@@ -3442,7 +3498,9 @@
       <c r="C32" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2">
+        <v>375</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1" t="s">
@@ -3454,7 +3512,9 @@
       <c r="C33" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2">
+        <v>440</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1" t="s">
@@ -3466,7 +3526,9 @@
       <c r="C34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2">
+        <v>440</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="1" t="s">
@@ -3478,7 +3540,9 @@
       <c r="C35" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2">
+        <v>440</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="1" t="s">
@@ -3490,7 +3554,9 @@
       <c r="C36" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="2">
+        <v>650</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="1" t="s">
@@ -3502,7 +3568,9 @@
       <c r="C37" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D37" s="2"/>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="1" t="s">
@@ -3512,7 +3580,9 @@
       <c r="C38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D38" s="2"/>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="1" t="s">
@@ -3524,7 +3594,9 @@
       <c r="C39" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="D39" s="2">
+        <v>58</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="1" t="s">
@@ -3536,7 +3608,9 @@
       <c r="C40" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="D40" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="1" t="s">
@@ -3548,7 +3622,9 @@
       <c r="C41" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D41" s="2"/>
+      <c r="D41" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="1" t="s">
@@ -3560,7 +3636,9 @@
       <c r="C42" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D42" s="2"/>
+      <c r="D42" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="1" t="s">
@@ -3572,7 +3650,9 @@
       <c r="C43" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D43" s="2"/>
+      <c r="D43" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="1" t="s">
@@ -3584,7 +3664,9 @@
       <c r="C44" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="2"/>
+      <c r="D44" s="2">
+        <v>52</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="1" t="s">
@@ -3596,7 +3678,9 @@
       <c r="C45" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D45" s="2"/>
+      <c r="D45" s="2">
+        <v>52</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="1" t="s">
@@ -3608,7 +3692,9 @@
       <c r="C46" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D46" s="2"/>
+      <c r="D46" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="1" t="s">
@@ -3620,7 +3706,9 @@
       <c r="C47" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="2"/>
+      <c r="D47" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="1" t="s">
@@ -3632,7 +3720,9 @@
       <c r="C48" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D48" s="2"/>
+      <c r="D48" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="1" t="s">
@@ -3644,7 +3734,9 @@
       <c r="C49" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D49" s="2"/>
+      <c r="D49" s="2">
+        <v>68</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="1" t="s">
@@ -3656,7 +3748,9 @@
       <c r="C50" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D50" s="2"/>
+      <c r="D50" s="2">
+        <v>19</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="1" t="s">
@@ -3668,7 +3762,9 @@
       <c r="C51" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D51" s="2"/>
+      <c r="D51" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="1" t="s">
@@ -3680,7 +3776,9 @@
       <c r="C52" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D52" s="2"/>
+      <c r="D52" s="2">
+        <v>48</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="1" t="s">
@@ -3692,7 +3790,9 @@
       <c r="C53" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="2">
+        <v>48</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="1" t="s">
@@ -3704,7 +3804,9 @@
       <c r="C54" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D54" s="2"/>
+      <c r="D54" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="1" t="s">
@@ -3716,7 +3818,9 @@
       <c r="C55" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D55" s="2"/>
+      <c r="D55" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="1" t="s">
@@ -3728,7 +3832,9 @@
       <c r="C56" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D56" s="2"/>
+      <c r="D56" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="1" t="s">
@@ -3740,7 +3846,9 @@
       <c r="C57" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D57" s="2"/>
+      <c r="D57" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="1" t="s">
@@ -3752,7 +3860,9 @@
       <c r="C58" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="1" t="s">
@@ -3764,7 +3874,9 @@
       <c r="C59" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D59" s="2"/>
+      <c r="D59" s="2">
+        <v>64</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="1" t="s">
@@ -3774,7 +3886,9 @@
       <c r="C60" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D60" s="2"/>
+      <c r="D60" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="1" t="s">
@@ -3784,7 +3898,9 @@
       <c r="C61" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D61" s="2"/>
+      <c r="D61" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="1" t="s">
@@ -3796,7 +3912,9 @@
       <c r="C62" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D62" s="2"/>
+      <c r="D62" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="1" t="s">
@@ -3808,7 +3926,9 @@
       <c r="C63" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D63" s="2"/>
+      <c r="D63" s="2">
+        <v>19</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="1" t="s">
@@ -3820,7 +3940,9 @@
       <c r="C64" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D64" s="2"/>
+      <c r="D64" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="1" t="s">
@@ -3832,7 +3954,9 @@
       <c r="C65" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D65" s="2"/>
+      <c r="D65" s="2">
+        <v>172</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="1" t="s">
@@ -3844,7 +3968,9 @@
       <c r="C66" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D66" s="2"/>
+      <c r="D66" s="2">
+        <v>210</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="1" t="s">
@@ -3856,7 +3982,9 @@
       <c r="C67" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D67" s="2"/>
+      <c r="D67" s="2">
+        <v>220</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="1" t="s">
@@ -3868,7 +3996,9 @@
       <c r="C68" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D68" s="2"/>
+      <c r="D68" s="2">
+        <v>230</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="1" t="s">
@@ -3880,7 +4010,9 @@
       <c r="C69" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D69" s="2"/>
+      <c r="D69" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="1" t="s">
@@ -3892,7 +4024,9 @@
       <c r="C70" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D70" s="2"/>
+      <c r="D70" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="1" t="s">
@@ -3904,7 +4038,9 @@
       <c r="C71" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D71" s="2"/>
+      <c r="D71" s="2">
+        <v>82</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="1" t="s">
@@ -3916,7 +4052,9 @@
       <c r="C72" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D72" s="2"/>
+      <c r="D72" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="1" t="s">
@@ -3928,7 +4066,9 @@
       <c r="C73" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D73" s="2"/>
+      <c r="D73" s="2">
+        <v>112</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="1" t="s">
@@ -3940,7 +4080,9 @@
       <c r="C74" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D74" s="2"/>
+      <c r="D74" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="1" t="s">
@@ -3952,7 +4094,9 @@
       <c r="C75" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D75" s="2"/>
+      <c r="D75" s="2">
+        <v>189</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="1" t="s">
@@ -3964,7 +4108,9 @@
       <c r="C76" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D76" s="2"/>
+      <c r="D76" s="2">
+        <v>106</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="1" t="s">
@@ -3976,7 +4122,9 @@
       <c r="C77" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="D77" s="2"/>
+      <c r="D77" s="2">
+        <v>136</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="1" t="s">
@@ -3988,7 +4136,9 @@
       <c r="C78" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D78" s="2"/>
+      <c r="D78" s="2">
+        <v>131</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="1" t="s">
@@ -4000,7 +4150,9 @@
       <c r="C79" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D79" s="2"/>
+      <c r="D79" s="2">
+        <v>189</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="1" t="s">
@@ -4012,7 +4164,9 @@
       <c r="C80" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D80" s="2"/>
+      <c r="D80" s="2">
+        <v>130</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="1" t="s">
@@ -4024,7 +4178,9 @@
       <c r="C81" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D81" s="2"/>
+      <c r="D81" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="1" t="s">
@@ -4036,7 +4192,9 @@
       <c r="C82" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D82" s="2"/>
+      <c r="D82" s="2">
+        <v>149</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="1" t="s">
@@ -4048,7 +4206,9 @@
       <c r="C83" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D83" s="2"/>
+      <c r="D83" s="2">
+        <v>149</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="1" t="s">
@@ -4060,7 +4220,9 @@
       <c r="C84" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D84" s="2"/>
+      <c r="D84" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="1" t="s">
@@ -4072,7 +4234,9 @@
       <c r="C85" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D85" s="2"/>
+      <c r="D85" s="2">
+        <v>149</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="1" t="s">
@@ -4084,7 +4248,9 @@
       <c r="C86" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D86" s="2"/>
+      <c r="D86" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="1" t="s">
@@ -4096,7 +4262,9 @@
       <c r="C87" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D87" s="2"/>
+      <c r="D87" s="2">
+        <v>145</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="1" t="s">
@@ -4108,7 +4276,9 @@
       <c r="C88" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D88" s="2"/>
+      <c r="D88" s="2">
+        <v>145</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="1" t="s">
@@ -4120,7 +4290,9 @@
       <c r="C89" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D89" s="2"/>
+      <c r="D89" s="2">
+        <v>130</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="1" t="s">
@@ -4132,7 +4304,9 @@
       <c r="C90" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D90" s="2"/>
+      <c r="D90" s="2">
+        <v>189</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="1" t="s">
@@ -4144,7 +4318,9 @@
       <c r="C91" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D91" s="2"/>
+      <c r="D91" s="2">
+        <v>220</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="1" t="s">
@@ -4156,7 +4332,9 @@
       <c r="C92" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D92" s="2"/>
+      <c r="D92" s="2">
+        <v>149</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="1" t="s">
@@ -4168,7 +4346,9 @@
       <c r="C93" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D93" s="2"/>
+      <c r="D93" s="2">
+        <v>149</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="1" t="s">
@@ -4180,7 +4360,9 @@
       <c r="C94" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="D94" s="2"/>
+      <c r="D94" s="2">
+        <v>189</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="1" t="s">
@@ -4192,7 +4374,9 @@
       <c r="C95" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D95" s="2"/>
+      <c r="D95" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="1" t="s">
@@ -4204,7 +4388,9 @@
       <c r="C96" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D96" s="2"/>
+      <c r="D96" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="1" t="s">
@@ -4216,7 +4402,9 @@
       <c r="C97" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D97" s="2"/>
+      <c r="D97" s="2">
+        <v>220</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="1" t="s">
@@ -4228,7 +4416,9 @@
       <c r="C98" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D98" s="2"/>
+      <c r="D98" s="2">
+        <v>366</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="1" t="s">
@@ -4240,7 +4430,9 @@
       <c r="C99" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D99" s="2"/>
+      <c r="D99" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="1" t="s">
@@ -4252,7 +4444,9 @@
       <c r="C100" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D100" s="2"/>
+      <c r="D100" s="2">
+        <v>660</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="1" t="s">
@@ -4264,7 +4458,9 @@
       <c r="C101" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D101" s="2"/>
+      <c r="D101" s="2">
+        <v>452</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="1" t="s">
@@ -4276,7 +4472,9 @@
       <c r="C102" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D102" s="2"/>
+      <c r="D102" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="1" t="s">
@@ -4288,7 +4486,9 @@
       <c r="C103" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D103" s="2"/>
+      <c r="D103" s="2">
+        <v>496</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="1" t="s">
@@ -4300,7 +4500,9 @@
       <c r="C104" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D104" s="2"/>
+      <c r="D104" s="2">
+        <v>660</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
       <c r="A105" s="1" t="s">
@@ -4312,7 +4514,9 @@
       <c r="C105" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D105" s="2"/>
+      <c r="D105" s="2">
+        <v>660</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
       <c r="A106" s="1" t="s">
@@ -4324,7 +4528,9 @@
       <c r="C106" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="D106" s="2"/>
+      <c r="D106" s="2">
+        <v>660</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
       <c r="A107" s="1" t="s">
@@ -4336,7 +4542,9 @@
       <c r="C107" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D107" s="2"/>
+      <c r="D107" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
       <c r="A108" s="1" t="s">
@@ -4348,7 +4556,9 @@
       <c r="C108" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="D108" s="2"/>
+      <c r="D108" s="2">
+        <v>524</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="1" t="s">
@@ -4360,7 +4570,9 @@
       <c r="C109" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="D109" s="2"/>
+      <c r="D109" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="1" t="s">
@@ -4372,7 +4584,9 @@
       <c r="C110" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="D110" s="2"/>
+      <c r="D110" s="2">
+        <v>550</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="1" t="s">
@@ -4384,7 +4598,9 @@
       <c r="C111" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D111" s="2"/>
+      <c r="D111" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="1" t="s">
@@ -4396,7 +4612,9 @@
       <c r="C112" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="D112" s="2"/>
+      <c r="D112" s="2">
+        <v>232</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
       <c r="A113" s="1" t="s">
@@ -4408,7 +4626,9 @@
       <c r="C113" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="D113" s="2"/>
+      <c r="D113" s="2">
+        <v>200</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
       <c r="A114" s="1" t="s">
@@ -4420,7 +4640,9 @@
       <c r="C114" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="D114" s="2"/>
+      <c r="D114" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
       <c r="A115" s="1" t="s">
@@ -4432,7 +4654,9 @@
       <c r="C115" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="D115" s="2"/>
+      <c r="D115" s="2">
+        <v>243</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
       <c r="A116" s="1" t="s">
@@ -4444,7 +4668,9 @@
       <c r="C116" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="D116" s="2"/>
+      <c r="D116" s="2">
+        <v>224</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
       <c r="A117" s="1" t="s">
@@ -4456,7 +4682,9 @@
       <c r="C117" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="D117" s="2"/>
+      <c r="D117" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
       <c r="A118" s="1" t="s">
@@ -4468,7 +4696,9 @@
       <c r="C118" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="D118" s="2"/>
+      <c r="D118" s="2">
+        <v>269</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
       <c r="A119" s="1" t="s">
@@ -4480,7 +4710,9 @@
       <c r="C119" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="D119" s="2"/>
+      <c r="D119" s="2">
+        <v>269</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
       <c r="A120" s="1" t="s">
@@ -4492,7 +4724,9 @@
       <c r="C120" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D120" s="2"/>
+      <c r="D120" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
       <c r="A121" s="1" t="s">
@@ -4504,7 +4738,9 @@
       <c r="C121" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D121" s="2"/>
+      <c r="D121" s="2">
+        <v>245</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
       <c r="A122" s="1" t="s">
@@ -4516,7 +4752,9 @@
       <c r="C122" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="D122" s="2"/>
+      <c r="D122" s="2">
+        <v>440</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
       <c r="A123" s="1" t="s">
@@ -4528,7 +4766,9 @@
       <c r="C123" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="D123" s="2"/>
+      <c r="D123" s="2">
+        <v>550</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
       <c r="A124" s="1" t="s">
@@ -4540,7 +4780,9 @@
       <c r="C124" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="D124" s="2"/>
+      <c r="D124" s="2">
+        <v>426</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
       <c r="A125" s="1" t="s">
@@ -4552,7 +4794,9 @@
       <c r="C125" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="D125" s="2"/>
+      <c r="D125" s="2">
+        <v>426</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
       <c r="A126" s="1" t="s">
@@ -4564,7 +4808,9 @@
       <c r="C126" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="D126" s="2"/>
+      <c r="D126" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
       <c r="A127" s="1" t="s">
@@ -4576,7 +4822,9 @@
       <c r="C127" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="D127" s="2"/>
+      <c r="D127" s="2">
+        <v>440</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
       <c r="A128" s="1" t="s">
@@ -4588,7 +4836,9 @@
       <c r="C128" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="D128" s="2"/>
+      <c r="D128" s="2">
+        <v>550</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
       <c r="A129" s="1" t="s">
@@ -4600,7 +4850,9 @@
       <c r="C129" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="D129" s="2"/>
+      <c r="D129" s="2">
+        <v>290</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
       <c r="A130" s="1" t="s">
@@ -4612,7 +4864,9 @@
       <c r="C130" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D130" s="2"/>
+      <c r="D130" s="2">
+        <v>296</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
       <c r="A131" s="1" t="s">
@@ -4624,7 +4878,9 @@
       <c r="C131" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="D131" s="2"/>
+      <c r="D131" s="2">
+        <v>330</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
       <c r="A132" s="1" t="s">
@@ -4636,7 +4892,9 @@
       <c r="C132" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D132" s="2"/>
+      <c r="D132" s="2">
+        <v>119</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
       <c r="A133" s="1" t="s">
@@ -4800,9 +5058,7 @@
       <c r="C144" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="D144" s="2">
-        <v>10</v>
-      </c>
+      <c r="D144" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
       <c r="A145" s="1" t="s">
@@ -4814,9 +5070,7 @@
       <c r="C145" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="D145" s="2">
-        <v>0</v>
-      </c>
+      <c r="D145" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
       <c r="A146" s="1" t="s">
@@ -4828,9 +5082,7 @@
       <c r="C146" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D146" s="2">
-        <v>14</v>
-      </c>
+      <c r="D146" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
       <c r="A147" s="1" t="s">

</xml_diff>

<commit_message>
three aircraft information was missing
</commit_message>
<xml_diff>
--- a/AIRCRAFTS.xlsx
+++ b/AIRCRAFTS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c0002738dae3070/Bureaublad/Study/Master/BigData/MBD_11/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gulbe\Documents\MBD\MBD_11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_50AAC5C78C2C8049B5ECEA08E7DECBB57FD71FC0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{643FC947-2BE2-4815-96B6-5BC309480898}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BE47C9-5F96-4CE5-9A78-AF3EC7C7DCF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="22110" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICAO aircraft type designators" sheetId="1" r:id="rId1"/>
@@ -2260,19 +2260,19 @@
   </sheetPr>
   <dimension ref="A1:D331"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>620</v>
       </c>
@@ -2284,7 +2284,7 @@
       </c>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2296,7 +2296,7 @@
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2320,7 +2320,7 @@
       </c>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2332,7 +2332,7 @@
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2368,7 +2368,7 @@
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2380,7 +2380,7 @@
       </c>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2392,7 +2392,7 @@
       </c>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2404,7 +2404,7 @@
       </c>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2440,7 +2440,7 @@
       </c>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="D16"/>
     </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="D17"/>
     </row>
-    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2488,7 +2488,7 @@
       </c>
       <c r="D18"/>
     </row>
-    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -2512,7 +2512,7 @@
       </c>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -2548,7 +2548,7 @@
       </c>
       <c r="D23"/>
     </row>
-    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -2560,7 +2560,7 @@
       </c>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -2584,7 +2584,7 @@
       </c>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -2596,7 +2596,7 @@
       </c>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -2620,7 +2620,7 @@
       </c>
       <c r="D29"/>
     </row>
-    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -2632,7 +2632,7 @@
       </c>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -2644,7 +2644,7 @@
       </c>
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="D32"/>
     </row>
-    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -2680,7 +2680,7 @@
       </c>
       <c r="D34"/>
     </row>
-    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -2692,7 +2692,7 @@
       </c>
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>62</v>
       </c>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -2716,7 +2716,7 @@
       </c>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>66</v>
       </c>
@@ -2728,7 +2728,7 @@
       </c>
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -2752,7 +2752,7 @@
       </c>
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -2764,7 +2764,7 @@
       </c>
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -2776,7 +2776,7 @@
       </c>
       <c r="D42"/>
     </row>
-    <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>76</v>
       </c>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="D43"/>
     </row>
-    <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -2800,7 +2800,7 @@
       </c>
       <c r="D44"/>
     </row>
-    <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -2812,7 +2812,7 @@
       </c>
       <c r="D45"/>
     </row>
-    <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -2824,7 +2824,7 @@
       </c>
       <c r="D46"/>
     </row>
-    <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="D47"/>
     </row>
-    <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="D48"/>
     </row>
-    <row r="49" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="D49"/>
     </row>
-    <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>90</v>
       </c>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="D50"/>
     </row>
-    <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>92</v>
       </c>
@@ -2884,7 +2884,7 @@
       </c>
       <c r="D51"/>
     </row>
-    <row r="52" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>94</v>
       </c>
@@ -2896,7 +2896,7 @@
       </c>
       <c r="D52"/>
     </row>
-    <row r="53" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>96</v>
       </c>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="D53"/>
     </row>
-    <row r="54" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>98</v>
       </c>
@@ -2920,7 +2920,7 @@
       </c>
       <c r="D54"/>
     </row>
-    <row r="55" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>100</v>
       </c>
@@ -2932,7 +2932,7 @@
       </c>
       <c r="D55"/>
     </row>
-    <row r="56" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>102</v>
       </c>
@@ -2944,7 +2944,7 @@
       </c>
       <c r="D56"/>
     </row>
-    <row r="57" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>104</v>
       </c>
@@ -2956,7 +2956,7 @@
       </c>
       <c r="D57"/>
     </row>
-    <row r="58" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>106</v>
       </c>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="D58"/>
     </row>
-    <row r="59" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>108</v>
       </c>
@@ -2980,7 +2980,7 @@
       </c>
       <c r="D59"/>
     </row>
-    <row r="60" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>110</v>
       </c>
@@ -2992,7 +2992,7 @@
       </c>
       <c r="D60"/>
     </row>
-    <row r="61" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>112</v>
       </c>
@@ -3004,7 +3004,7 @@
       </c>
       <c r="D61"/>
     </row>
-    <row r="62" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>114</v>
       </c>
@@ -3016,7 +3016,7 @@
       </c>
       <c r="D62"/>
     </row>
-    <row r="63" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>116</v>
       </c>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="D63"/>
     </row>
-    <row r="64" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>118</v>
       </c>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="D64"/>
     </row>
-    <row r="65" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>120</v>
       </c>
@@ -3052,7 +3052,7 @@
       </c>
       <c r="D65"/>
     </row>
-    <row r="66" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>122</v>
       </c>
@@ -3064,7 +3064,7 @@
       </c>
       <c r="D66"/>
     </row>
-    <row r="67" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>124</v>
       </c>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="D67"/>
     </row>
-    <row r="68" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>126</v>
       </c>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="D68"/>
     </row>
-    <row r="69" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>128</v>
       </c>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="D69"/>
     </row>
-    <row r="70" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>130</v>
       </c>
@@ -3112,7 +3112,7 @@
       </c>
       <c r="D70"/>
     </row>
-    <row r="71" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>132</v>
       </c>
@@ -3124,7 +3124,7 @@
       </c>
       <c r="D71"/>
     </row>
-    <row r="72" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>134</v>
       </c>
@@ -3136,7 +3136,7 @@
       </c>
       <c r="D72"/>
     </row>
-    <row r="73" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>136</v>
       </c>
@@ -3148,7 +3148,7 @@
       </c>
       <c r="D73"/>
     </row>
-    <row r="74" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>138</v>
       </c>
@@ -3160,7 +3160,7 @@
       </c>
       <c r="D74"/>
     </row>
-    <row r="75" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>140</v>
       </c>
@@ -3172,7 +3172,7 @@
       </c>
       <c r="D75"/>
     </row>
-    <row r="76" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>142</v>
       </c>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="D76"/>
     </row>
-    <row r="77" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>144</v>
       </c>
@@ -3196,7 +3196,7 @@
       </c>
       <c r="D77"/>
     </row>
-    <row r="78" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>146</v>
       </c>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="D78"/>
     </row>
-    <row r="79" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>148</v>
       </c>
@@ -3220,7 +3220,7 @@
       </c>
       <c r="D79"/>
     </row>
-    <row r="80" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>150</v>
       </c>
@@ -3232,7 +3232,7 @@
       </c>
       <c r="D80"/>
     </row>
-    <row r="81" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>150</v>
       </c>
@@ -3244,7 +3244,7 @@
       </c>
       <c r="D81"/>
     </row>
-    <row r="82" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>153</v>
       </c>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="D82"/>
     </row>
-    <row r="83" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>153</v>
       </c>
@@ -3268,7 +3268,7 @@
       </c>
       <c r="D83"/>
     </row>
-    <row r="84" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>153</v>
       </c>
@@ -3280,7 +3280,7 @@
       </c>
       <c r="D84"/>
     </row>
-    <row r="85" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>157</v>
       </c>
@@ -3292,7 +3292,7 @@
       </c>
       <c r="D85"/>
     </row>
-    <row r="86" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>157</v>
       </c>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="D86"/>
     </row>
-    <row r="87" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>160</v>
       </c>
@@ -3316,7 +3316,7 @@
       </c>
       <c r="D87"/>
     </row>
-    <row r="88" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>160</v>
       </c>
@@ -3328,7 +3328,7 @@
       </c>
       <c r="D88"/>
     </row>
-    <row r="89" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>163</v>
       </c>
@@ -3340,7 +3340,7 @@
       </c>
       <c r="D89"/>
     </row>
-    <row r="90" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>165</v>
       </c>
@@ -3352,7 +3352,7 @@
       </c>
       <c r="D90"/>
     </row>
-    <row r="91" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>167</v>
       </c>
@@ -3364,7 +3364,7 @@
       </c>
       <c r="D91"/>
     </row>
-    <row r="92" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>169</v>
       </c>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>169</v>
       </c>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="D93"/>
     </row>
-    <row r="94" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>165</v>
       </c>
@@ -3400,7 +3400,7 @@
       </c>
       <c r="D94"/>
     </row>
-    <row r="95" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>165</v>
       </c>
@@ -3412,7 +3412,7 @@
       </c>
       <c r="D95"/>
     </row>
-    <row r="96" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>165</v>
       </c>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="D96"/>
     </row>
-    <row r="97" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>167</v>
       </c>
@@ -3436,7 +3436,7 @@
       </c>
       <c r="D97"/>
     </row>
-    <row r="98" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>176</v>
       </c>
@@ -3448,7 +3448,7 @@
       </c>
       <c r="D98"/>
     </row>
-    <row r="99" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>176</v>
       </c>
@@ -3460,7 +3460,7 @@
       </c>
       <c r="D99"/>
     </row>
-    <row r="100" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>179</v>
       </c>
@@ -3472,7 +3472,7 @@
       </c>
       <c r="D100"/>
     </row>
-    <row r="101" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>179</v>
       </c>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="D101"/>
     </row>
-    <row r="102" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>179</v>
       </c>
@@ -3496,7 +3496,7 @@
       </c>
       <c r="D102"/>
     </row>
-    <row r="103" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>183</v>
       </c>
@@ -3508,7 +3508,7 @@
       </c>
       <c r="D103"/>
     </row>
-    <row r="104" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>183</v>
       </c>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="D104"/>
     </row>
-    <row r="105" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>186</v>
       </c>
@@ -3532,7 +3532,7 @@
       </c>
       <c r="D105"/>
     </row>
-    <row r="106" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>186</v>
       </c>
@@ -3544,7 +3544,7 @@
       </c>
       <c r="D106"/>
     </row>
-    <row r="107" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>186</v>
       </c>
@@ -3556,7 +3556,7 @@
       </c>
       <c r="D107"/>
     </row>
-    <row r="108" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>190</v>
       </c>
@@ -3568,7 +3568,7 @@
       </c>
       <c r="D108"/>
     </row>
-    <row r="109" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>190</v>
       </c>
@@ -3580,7 +3580,7 @@
       </c>
       <c r="D109"/>
     </row>
-    <row r="110" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>193</v>
       </c>
@@ -3592,7 +3592,7 @@
       </c>
       <c r="D110"/>
     </row>
-    <row r="111" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>193</v>
       </c>
@@ -3604,7 +3604,7 @@
       </c>
       <c r="D111"/>
     </row>
-    <row r="112" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>196</v>
       </c>
@@ -3616,7 +3616,7 @@
       </c>
       <c r="D112"/>
     </row>
-    <row r="113" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>198</v>
       </c>
@@ -3628,7 +3628,7 @@
       </c>
       <c r="D113"/>
     </row>
-    <row r="114" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>198</v>
       </c>
@@ -3640,7 +3640,7 @@
       </c>
       <c r="D114"/>
     </row>
-    <row r="115" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>201</v>
       </c>
@@ -3652,7 +3652,7 @@
       </c>
       <c r="D115"/>
     </row>
-    <row r="116" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>203</v>
       </c>
@@ -3664,7 +3664,7 @@
       </c>
       <c r="D116"/>
     </row>
-    <row r="117" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>203</v>
       </c>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="D117"/>
     </row>
-    <row r="118" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>206</v>
       </c>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="D118"/>
     </row>
-    <row r="119" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>206</v>
       </c>
@@ -3700,7 +3700,7 @@
       </c>
       <c r="D119"/>
     </row>
-    <row r="120" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>206</v>
       </c>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D120"/>
     </row>
-    <row r="121" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>210</v>
       </c>
@@ -3724,7 +3724,7 @@
       </c>
       <c r="D121"/>
     </row>
-    <row r="122" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>212</v>
       </c>
@@ -3736,7 +3736,7 @@
       </c>
       <c r="D122"/>
     </row>
-    <row r="123" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>214</v>
       </c>
@@ -3748,7 +3748,7 @@
       </c>
       <c r="D123"/>
     </row>
-    <row r="124" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>216</v>
       </c>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="D124"/>
     </row>
-    <row r="125" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>218</v>
       </c>
@@ -3772,7 +3772,7 @@
       </c>
       <c r="D125"/>
     </row>
-    <row r="126" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>220</v>
       </c>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="D126"/>
     </row>
-    <row r="127" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>220</v>
       </c>
@@ -3796,7 +3796,7 @@
       </c>
       <c r="D127"/>
     </row>
-    <row r="128" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>223</v>
       </c>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="D128"/>
     </row>
-    <row r="129" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>225</v>
       </c>
@@ -3820,7 +3820,7 @@
       </c>
       <c r="D129"/>
     </row>
-    <row r="130" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>227</v>
       </c>
@@ -3832,7 +3832,7 @@
       </c>
       <c r="D130"/>
     </row>
-    <row r="131" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>229</v>
       </c>
@@ -3844,7 +3844,7 @@
       </c>
       <c r="D131"/>
     </row>
-    <row r="132" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>231</v>
       </c>
@@ -3856,7 +3856,7 @@
       </c>
       <c r="D132"/>
     </row>
-    <row r="133" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>233</v>
       </c>
@@ -3868,7 +3868,7 @@
       </c>
       <c r="D133"/>
     </row>
-    <row r="134" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>235</v>
       </c>
@@ -3880,7 +3880,7 @@
       </c>
       <c r="D134"/>
     </row>
-    <row r="135" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>237</v>
       </c>
@@ -3892,7 +3892,7 @@
       </c>
       <c r="D135"/>
     </row>
-    <row r="136" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>239</v>
       </c>
@@ -3904,7 +3904,7 @@
       </c>
       <c r="D136"/>
     </row>
-    <row r="137" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>241</v>
       </c>
@@ -3916,7 +3916,7 @@
       </c>
       <c r="D137"/>
     </row>
-    <row r="138" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>243</v>
       </c>
@@ -3928,7 +3928,7 @@
       </c>
       <c r="D138"/>
     </row>
-    <row r="139" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>245</v>
       </c>
@@ -3940,7 +3940,7 @@
       </c>
       <c r="D139"/>
     </row>
-    <row r="140" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>247</v>
       </c>
@@ -3952,7 +3952,7 @@
       </c>
       <c r="D140"/>
     </row>
-    <row r="141" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>249</v>
       </c>
@@ -3964,7 +3964,7 @@
       </c>
       <c r="D141"/>
     </row>
-    <row r="142" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>251</v>
       </c>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="D142"/>
     </row>
-    <row r="143" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>253</v>
       </c>
@@ -3988,37 +3988,43 @@
       </c>
       <c r="D143"/>
     </row>
-    <row r="144" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>255</v>
       </c>
       <c r="B144" t="s">
         <v>256</v>
       </c>
-      <c r="C144" s="1"/>
+      <c r="C144" s="1">
+        <v>9</v>
+      </c>
       <c r="D144"/>
     </row>
-    <row r="145" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>257</v>
       </c>
       <c r="B145" t="s">
         <v>258</v>
       </c>
-      <c r="C145" s="1"/>
+      <c r="C145" s="1">
+        <v>100</v>
+      </c>
       <c r="D145"/>
     </row>
-    <row r="146" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>259</v>
       </c>
       <c r="B146" t="s">
         <v>260</v>
       </c>
-      <c r="C146" s="1"/>
+      <c r="C146" s="1">
+        <v>9</v>
+      </c>
       <c r="D146"/>
     </row>
-    <row r="147" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>261</v>
       </c>
@@ -4030,7 +4036,7 @@
       </c>
       <c r="D147"/>
     </row>
-    <row r="148" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>263</v>
       </c>
@@ -4042,7 +4048,7 @@
       </c>
       <c r="D148"/>
     </row>
-    <row r="149" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>265</v>
       </c>
@@ -4054,7 +4060,7 @@
       </c>
       <c r="D149"/>
     </row>
-    <row r="150" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>267</v>
       </c>
@@ -4066,7 +4072,7 @@
       </c>
       <c r="D150"/>
     </row>
-    <row r="151" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>269</v>
       </c>
@@ -4078,7 +4084,7 @@
       </c>
       <c r="D151"/>
     </row>
-    <row r="152" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>271</v>
       </c>
@@ -4090,7 +4096,7 @@
       </c>
       <c r="D152"/>
     </row>
-    <row r="153" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>273</v>
       </c>
@@ -4102,7 +4108,7 @@
       </c>
       <c r="D153"/>
     </row>
-    <row r="154" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>275</v>
       </c>
@@ -4114,7 +4120,7 @@
       </c>
       <c r="D154"/>
     </row>
-    <row r="155" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>277</v>
       </c>
@@ -4126,7 +4132,7 @@
       </c>
       <c r="D155"/>
     </row>
-    <row r="156" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>279</v>
       </c>
@@ -4138,7 +4144,7 @@
       </c>
       <c r="D156"/>
     </row>
-    <row r="157" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>281</v>
       </c>
@@ -4150,7 +4156,7 @@
       </c>
       <c r="D157"/>
     </row>
-    <row r="158" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>283</v>
       </c>
@@ -4162,7 +4168,7 @@
       </c>
       <c r="D158"/>
     </row>
-    <row r="159" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>285</v>
       </c>
@@ -4174,7 +4180,7 @@
       </c>
       <c r="D159"/>
     </row>
-    <row r="160" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>287</v>
       </c>
@@ -4186,7 +4192,7 @@
       </c>
       <c r="D160"/>
     </row>
-    <row r="161" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>289</v>
       </c>
@@ -4198,7 +4204,7 @@
       </c>
       <c r="D161"/>
     </row>
-    <row r="162" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>291</v>
       </c>
@@ -4210,7 +4216,7 @@
       </c>
       <c r="D162"/>
     </row>
-    <row r="163" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>293</v>
       </c>
@@ -4222,7 +4228,7 @@
       </c>
       <c r="D163"/>
     </row>
-    <row r="164" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>295</v>
       </c>
@@ -4234,7 +4240,7 @@
       </c>
       <c r="D164"/>
     </row>
-    <row r="165" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>297</v>
       </c>
@@ -4246,7 +4252,7 @@
       </c>
       <c r="D165"/>
     </row>
-    <row r="166" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>299</v>
       </c>
@@ -4258,7 +4264,7 @@
       </c>
       <c r="D166"/>
     </row>
-    <row r="167" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>301</v>
       </c>
@@ -4270,7 +4276,7 @@
       </c>
       <c r="D167"/>
     </row>
-    <row r="168" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>303</v>
       </c>
@@ -4282,7 +4288,7 @@
       </c>
       <c r="D168"/>
     </row>
-    <row r="169" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>305</v>
       </c>
@@ -4294,7 +4300,7 @@
       </c>
       <c r="D169"/>
     </row>
-    <row r="170" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>307</v>
       </c>
@@ -4306,7 +4312,7 @@
       </c>
       <c r="D170"/>
     </row>
-    <row r="171" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>309</v>
       </c>
@@ -4318,7 +4324,7 @@
       </c>
       <c r="D171"/>
     </row>
-    <row r="172" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>311</v>
       </c>
@@ -4330,7 +4336,7 @@
       </c>
       <c r="D172"/>
     </row>
-    <row r="173" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>313</v>
       </c>
@@ -4342,7 +4348,7 @@
       </c>
       <c r="D173"/>
     </row>
-    <row r="174" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>315</v>
       </c>
@@ -4354,7 +4360,7 @@
       </c>
       <c r="D174"/>
     </row>
-    <row r="175" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>317</v>
       </c>
@@ -4366,7 +4372,7 @@
       </c>
       <c r="D175"/>
     </row>
-    <row r="176" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>319</v>
       </c>
@@ -4378,7 +4384,7 @@
       </c>
       <c r="D176"/>
     </row>
-    <row r="177" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>321</v>
       </c>
@@ -4390,7 +4396,7 @@
       </c>
       <c r="D177"/>
     </row>
-    <row r="178" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>323</v>
       </c>
@@ -4402,7 +4408,7 @@
       </c>
       <c r="D178"/>
     </row>
-    <row r="179" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>325</v>
       </c>
@@ -4414,7 +4420,7 @@
       </c>
       <c r="D179"/>
     </row>
-    <row r="180" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>327</v>
       </c>
@@ -4426,7 +4432,7 @@
       </c>
       <c r="D180"/>
     </row>
-    <row r="181" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>329</v>
       </c>
@@ -4438,7 +4444,7 @@
       </c>
       <c r="D181"/>
     </row>
-    <row r="182" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>331</v>
       </c>
@@ -4450,7 +4456,7 @@
       </c>
       <c r="D182"/>
     </row>
-    <row r="183" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>331</v>
       </c>
@@ -4462,7 +4468,7 @@
       </c>
       <c r="D183"/>
     </row>
-    <row r="184" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>331</v>
       </c>
@@ -4474,7 +4480,7 @@
       </c>
       <c r="D184"/>
     </row>
-    <row r="185" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>331</v>
       </c>
@@ -4486,7 +4492,7 @@
       </c>
       <c r="D185"/>
     </row>
-    <row r="186" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>331</v>
       </c>
@@ -4498,7 +4504,7 @@
       </c>
       <c r="D186"/>
     </row>
-    <row r="187" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>337</v>
       </c>
@@ -4510,7 +4516,7 @@
       </c>
       <c r="D187"/>
     </row>
-    <row r="188" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>339</v>
       </c>
@@ -4522,7 +4528,7 @@
       </c>
       <c r="D188"/>
     </row>
-    <row r="189" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>341</v>
       </c>
@@ -4534,7 +4540,7 @@
       </c>
       <c r="D189"/>
     </row>
-    <row r="190" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>343</v>
       </c>
@@ -4546,7 +4552,7 @@
       </c>
       <c r="D190"/>
     </row>
-    <row r="191" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>345</v>
       </c>
@@ -4558,7 +4564,7 @@
       </c>
       <c r="D191"/>
     </row>
-    <row r="192" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>347</v>
       </c>
@@ -4570,7 +4576,7 @@
       </c>
       <c r="D192"/>
     </row>
-    <row r="193" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>349</v>
       </c>
@@ -4582,7 +4588,7 @@
       </c>
       <c r="D193"/>
     </row>
-    <row r="194" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>351</v>
       </c>
@@ -4594,7 +4600,7 @@
       </c>
       <c r="D194"/>
     </row>
-    <row r="195" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>353</v>
       </c>
@@ -4606,7 +4612,7 @@
       </c>
       <c r="D195"/>
     </row>
-    <row r="196" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>355</v>
       </c>
@@ -4618,7 +4624,7 @@
       </c>
       <c r="D196"/>
     </row>
-    <row r="197" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>357</v>
       </c>
@@ -4630,7 +4636,7 @@
       </c>
       <c r="D197"/>
     </row>
-    <row r="198" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>359</v>
       </c>
@@ -4642,7 +4648,7 @@
       </c>
       <c r="D198"/>
     </row>
-    <row r="199" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>361</v>
       </c>
@@ -4654,7 +4660,7 @@
       </c>
       <c r="D199"/>
     </row>
-    <row r="200" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>363</v>
       </c>
@@ -4666,7 +4672,7 @@
       </c>
       <c r="D200"/>
     </row>
-    <row r="201" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>365</v>
       </c>
@@ -4678,7 +4684,7 @@
       </c>
       <c r="D201"/>
     </row>
-    <row r="202" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>367</v>
       </c>
@@ -4690,7 +4696,7 @@
       </c>
       <c r="D202"/>
     </row>
-    <row r="203" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>369</v>
       </c>
@@ -4702,7 +4708,7 @@
       </c>
       <c r="D203"/>
     </row>
-    <row r="204" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>371</v>
       </c>
@@ -4714,7 +4720,7 @@
       </c>
       <c r="D204"/>
     </row>
-    <row r="205" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>373</v>
       </c>
@@ -4726,7 +4732,7 @@
       </c>
       <c r="D205"/>
     </row>
-    <row r="206" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>375</v>
       </c>
@@ -4738,7 +4744,7 @@
       </c>
       <c r="D206"/>
     </row>
-    <row r="207" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>377</v>
       </c>
@@ -4750,7 +4756,7 @@
       </c>
       <c r="D207"/>
     </row>
-    <row r="208" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>379</v>
       </c>
@@ -4762,7 +4768,7 @@
       </c>
       <c r="D208"/>
     </row>
-    <row r="209" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>381</v>
       </c>
@@ -4774,7 +4780,7 @@
       </c>
       <c r="D209"/>
     </row>
-    <row r="210" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>381</v>
       </c>
@@ -4786,7 +4792,7 @@
       </c>
       <c r="D210"/>
     </row>
-    <row r="211" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>384</v>
       </c>
@@ -4798,7 +4804,7 @@
       </c>
       <c r="D211"/>
     </row>
-    <row r="212" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>386</v>
       </c>
@@ -4810,7 +4816,7 @@
       </c>
       <c r="D212"/>
     </row>
-    <row r="213" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>388</v>
       </c>
@@ -4822,7 +4828,7 @@
       </c>
       <c r="D213"/>
     </row>
-    <row r="214" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>390</v>
       </c>
@@ -4834,7 +4840,7 @@
       </c>
       <c r="D214"/>
     </row>
-    <row r="215" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>392</v>
       </c>
@@ -4846,7 +4852,7 @@
       </c>
       <c r="D215"/>
     </row>
-    <row r="216" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>394</v>
       </c>
@@ -4858,7 +4864,7 @@
       </c>
       <c r="D216"/>
     </row>
-    <row r="217" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>396</v>
       </c>
@@ -4870,7 +4876,7 @@
       </c>
       <c r="D217"/>
     </row>
-    <row r="218" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>398</v>
       </c>
@@ -4882,7 +4888,7 @@
       </c>
       <c r="D218"/>
     </row>
-    <row r="219" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>400</v>
       </c>
@@ -4894,7 +4900,7 @@
       </c>
       <c r="D219"/>
     </row>
-    <row r="220" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>402</v>
       </c>
@@ -4906,7 +4912,7 @@
       </c>
       <c r="D220"/>
     </row>
-    <row r="221" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>404</v>
       </c>
@@ -4918,7 +4924,7 @@
       </c>
       <c r="D221"/>
     </row>
-    <row r="222" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>406</v>
       </c>
@@ -4930,7 +4936,7 @@
       </c>
       <c r="D222"/>
     </row>
-    <row r="223" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>408</v>
       </c>
@@ -4942,7 +4948,7 @@
       </c>
       <c r="D223"/>
     </row>
-    <row r="224" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>410</v>
       </c>
@@ -4954,7 +4960,7 @@
       </c>
       <c r="D224"/>
     </row>
-    <row r="225" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>412</v>
       </c>
@@ -4966,7 +4972,7 @@
       </c>
       <c r="D225"/>
     </row>
-    <row r="226" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>414</v>
       </c>
@@ -4978,7 +4984,7 @@
       </c>
       <c r="D226"/>
     </row>
-    <row r="227" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>416</v>
       </c>
@@ -4990,7 +4996,7 @@
       </c>
       <c r="D227"/>
     </row>
-    <row r="228" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>418</v>
       </c>
@@ -5002,7 +5008,7 @@
       </c>
       <c r="D228"/>
     </row>
-    <row r="229" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>420</v>
       </c>
@@ -5014,7 +5020,7 @@
       </c>
       <c r="D229"/>
     </row>
-    <row r="230" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>422</v>
       </c>
@@ -5026,7 +5032,7 @@
       </c>
       <c r="D230"/>
     </row>
-    <row r="231" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>424</v>
       </c>
@@ -5038,7 +5044,7 @@
       </c>
       <c r="D231"/>
     </row>
-    <row r="232" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>426</v>
       </c>
@@ -5050,7 +5056,7 @@
       </c>
       <c r="D232"/>
     </row>
-    <row r="233" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>428</v>
       </c>
@@ -5062,7 +5068,7 @@
       </c>
       <c r="D233"/>
     </row>
-    <row r="234" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>430</v>
       </c>
@@ -5074,7 +5080,7 @@
       </c>
       <c r="D234"/>
     </row>
-    <row r="235" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>432</v>
       </c>
@@ -5086,7 +5092,7 @@
       </c>
       <c r="D235"/>
     </row>
-    <row r="236" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>434</v>
       </c>
@@ -5098,7 +5104,7 @@
       </c>
       <c r="D236"/>
     </row>
-    <row r="237" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>436</v>
       </c>
@@ -5110,7 +5116,7 @@
       </c>
       <c r="D237"/>
     </row>
-    <row r="238" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>438</v>
       </c>
@@ -5122,7 +5128,7 @@
       </c>
       <c r="D238"/>
     </row>
-    <row r="239" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>440</v>
       </c>
@@ -5134,7 +5140,7 @@
       </c>
       <c r="D239"/>
     </row>
-    <row r="240" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>442</v>
       </c>
@@ -5146,7 +5152,7 @@
       </c>
       <c r="D240"/>
     </row>
-    <row r="241" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>444</v>
       </c>
@@ -5158,7 +5164,7 @@
       </c>
       <c r="D241"/>
     </row>
-    <row r="242" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>446</v>
       </c>
@@ -5170,7 +5176,7 @@
       </c>
       <c r="D242"/>
     </row>
-    <row r="243" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>448</v>
       </c>
@@ -5182,7 +5188,7 @@
       </c>
       <c r="D243"/>
     </row>
-    <row r="244" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>450</v>
       </c>
@@ -5194,7 +5200,7 @@
       </c>
       <c r="D244"/>
     </row>
-    <row r="245" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>452</v>
       </c>
@@ -5206,7 +5212,7 @@
       </c>
       <c r="D245"/>
     </row>
-    <row r="246" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>454</v>
       </c>
@@ -5218,7 +5224,7 @@
       </c>
       <c r="D246"/>
     </row>
-    <row r="247" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>456</v>
       </c>
@@ -5230,7 +5236,7 @@
       </c>
       <c r="D247"/>
     </row>
-    <row r="248" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>458</v>
       </c>
@@ -5242,7 +5248,7 @@
       </c>
       <c r="D248"/>
     </row>
-    <row r="249" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>460</v>
       </c>
@@ -5254,7 +5260,7 @@
       </c>
       <c r="D249"/>
     </row>
-    <row r="250" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>462</v>
       </c>
@@ -5266,7 +5272,7 @@
       </c>
       <c r="D250"/>
     </row>
-    <row r="251" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>464</v>
       </c>
@@ -5278,7 +5284,7 @@
       </c>
       <c r="D251"/>
     </row>
-    <row r="252" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>466</v>
       </c>
@@ -5290,7 +5296,7 @@
       </c>
       <c r="D252"/>
     </row>
-    <row r="253" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>468</v>
       </c>
@@ -5302,7 +5308,7 @@
       </c>
       <c r="D253"/>
     </row>
-    <row r="254" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>470</v>
       </c>
@@ -5314,7 +5320,7 @@
       </c>
       <c r="D254"/>
     </row>
-    <row r="255" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>472</v>
       </c>
@@ -5326,7 +5332,7 @@
       </c>
       <c r="D255"/>
     </row>
-    <row r="256" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>474</v>
       </c>
@@ -5338,7 +5344,7 @@
       </c>
       <c r="D256"/>
     </row>
-    <row r="257" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>476</v>
       </c>
@@ -5350,7 +5356,7 @@
       </c>
       <c r="D257"/>
     </row>
-    <row r="258" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>478</v>
       </c>
@@ -5362,7 +5368,7 @@
       </c>
       <c r="D258"/>
     </row>
-    <row r="259" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>480</v>
       </c>
@@ -5374,7 +5380,7 @@
       </c>
       <c r="D259"/>
     </row>
-    <row r="260" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>482</v>
       </c>
@@ -5386,7 +5392,7 @@
       </c>
       <c r="D260"/>
     </row>
-    <row r="261" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>484</v>
       </c>
@@ -5398,7 +5404,7 @@
       </c>
       <c r="D261"/>
     </row>
-    <row r="262" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>486</v>
       </c>
@@ -5410,7 +5416,7 @@
       </c>
       <c r="D262"/>
     </row>
-    <row r="263" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>488</v>
       </c>
@@ -5422,7 +5428,7 @@
       </c>
       <c r="D263"/>
     </row>
-    <row r="264" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>490</v>
       </c>
@@ -5434,7 +5440,7 @@
       </c>
       <c r="D264"/>
     </row>
-    <row r="265" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>492</v>
       </c>
@@ -5446,7 +5452,7 @@
       </c>
       <c r="D265"/>
     </row>
-    <row r="266" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>494</v>
       </c>
@@ -5458,7 +5464,7 @@
       </c>
       <c r="D266"/>
     </row>
-    <row r="267" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>496</v>
       </c>
@@ -5470,7 +5476,7 @@
       </c>
       <c r="D267"/>
     </row>
-    <row r="268" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>498</v>
       </c>
@@ -5482,7 +5488,7 @@
       </c>
       <c r="D268"/>
     </row>
-    <row r="269" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>500</v>
       </c>
@@ -5494,7 +5500,7 @@
       </c>
       <c r="D269"/>
     </row>
-    <row r="270" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>502</v>
       </c>
@@ -5506,7 +5512,7 @@
       </c>
       <c r="D270"/>
     </row>
-    <row r="271" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>504</v>
       </c>
@@ -5518,7 +5524,7 @@
       </c>
       <c r="D271"/>
     </row>
-    <row r="272" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>506</v>
       </c>
@@ -5530,7 +5536,7 @@
       </c>
       <c r="D272"/>
     </row>
-    <row r="273" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>508</v>
       </c>
@@ -5542,7 +5548,7 @@
       </c>
       <c r="D273"/>
     </row>
-    <row r="274" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>508</v>
       </c>
@@ -5554,7 +5560,7 @@
       </c>
       <c r="D274"/>
     </row>
-    <row r="275" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>508</v>
       </c>
@@ -5566,7 +5572,7 @@
       </c>
       <c r="D275"/>
     </row>
-    <row r="276" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>512</v>
       </c>
@@ -5578,7 +5584,7 @@
       </c>
       <c r="D276"/>
     </row>
-    <row r="277" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>514</v>
       </c>
@@ -5590,7 +5596,7 @@
       </c>
       <c r="D277"/>
     </row>
-    <row r="278" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>516</v>
       </c>
@@ -5602,7 +5608,7 @@
       </c>
       <c r="D278"/>
     </row>
-    <row r="279" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>518</v>
       </c>
@@ -5614,7 +5620,7 @@
       </c>
       <c r="D279"/>
     </row>
-    <row r="280" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>520</v>
       </c>
@@ -5626,7 +5632,7 @@
       </c>
       <c r="D280"/>
     </row>
-    <row r="281" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>522</v>
       </c>
@@ -5638,7 +5644,7 @@
       </c>
       <c r="D281"/>
     </row>
-    <row r="282" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>524</v>
       </c>
@@ -5650,7 +5656,7 @@
       </c>
       <c r="D282"/>
     </row>
-    <row r="283" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>526</v>
       </c>
@@ -5662,7 +5668,7 @@
       </c>
       <c r="D283"/>
     </row>
-    <row r="284" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>528</v>
       </c>
@@ -5674,7 +5680,7 @@
       </c>
       <c r="D284"/>
     </row>
-    <row r="285" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>530</v>
       </c>
@@ -5686,7 +5692,7 @@
       </c>
       <c r="D285"/>
     </row>
-    <row r="286" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>532</v>
       </c>
@@ -5698,7 +5704,7 @@
       </c>
       <c r="D286"/>
     </row>
-    <row r="287" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>534</v>
       </c>
@@ -5710,7 +5716,7 @@
       </c>
       <c r="D287"/>
     </row>
-    <row r="288" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>536</v>
       </c>
@@ -5722,7 +5728,7 @@
       </c>
       <c r="D288"/>
     </row>
-    <row r="289" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>538</v>
       </c>
@@ -5734,7 +5740,7 @@
       </c>
       <c r="D289"/>
     </row>
-    <row r="290" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>540</v>
       </c>
@@ -5746,7 +5752,7 @@
       </c>
       <c r="D290"/>
     </row>
-    <row r="291" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>542</v>
       </c>
@@ -5758,7 +5764,7 @@
       </c>
       <c r="D291"/>
     </row>
-    <row r="292" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>544</v>
       </c>
@@ -5770,7 +5776,7 @@
       </c>
       <c r="D292"/>
     </row>
-    <row r="293" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>546</v>
       </c>
@@ -5782,7 +5788,7 @@
       </c>
       <c r="D293"/>
     </row>
-    <row r="294" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>548</v>
       </c>
@@ -5794,7 +5800,7 @@
       </c>
       <c r="D294"/>
     </row>
-    <row r="295" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>550</v>
       </c>
@@ -5806,7 +5812,7 @@
       </c>
       <c r="D295"/>
     </row>
-    <row r="296" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>552</v>
       </c>
@@ -5818,7 +5824,7 @@
       </c>
       <c r="D296"/>
     </row>
-    <row r="297" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>554</v>
       </c>
@@ -5830,7 +5836,7 @@
       </c>
       <c r="D297"/>
     </row>
-    <row r="298" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>556</v>
       </c>
@@ -5842,7 +5848,7 @@
       </c>
       <c r="D298"/>
     </row>
-    <row r="299" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>558</v>
       </c>
@@ -5854,7 +5860,7 @@
       </c>
       <c r="D299"/>
     </row>
-    <row r="300" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>560</v>
       </c>
@@ -5866,7 +5872,7 @@
       </c>
       <c r="D300"/>
     </row>
-    <row r="301" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>562</v>
       </c>
@@ -5878,7 +5884,7 @@
       </c>
       <c r="D301"/>
     </row>
-    <row r="302" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>564</v>
       </c>
@@ -5890,7 +5896,7 @@
       </c>
       <c r="D302"/>
     </row>
-    <row r="303" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>566</v>
       </c>
@@ -5902,7 +5908,7 @@
       </c>
       <c r="D303"/>
     </row>
-    <row r="304" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>568</v>
       </c>
@@ -5914,7 +5920,7 @@
       </c>
       <c r="D304"/>
     </row>
-    <row r="305" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>570</v>
       </c>
@@ -5926,7 +5932,7 @@
       </c>
       <c r="D305"/>
     </row>
-    <row r="306" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>572</v>
       </c>
@@ -5938,7 +5944,7 @@
       </c>
       <c r="D306"/>
     </row>
-    <row r="307" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>574</v>
       </c>
@@ -5950,7 +5956,7 @@
       </c>
       <c r="D307"/>
     </row>
-    <row r="308" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>576</v>
       </c>
@@ -5962,7 +5968,7 @@
       </c>
       <c r="D308"/>
     </row>
-    <row r="309" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>578</v>
       </c>
@@ -5974,7 +5980,7 @@
       </c>
       <c r="D309"/>
     </row>
-    <row r="310" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>580</v>
       </c>
@@ -5986,7 +5992,7 @@
       </c>
       <c r="D310"/>
     </row>
-    <row r="311" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>582</v>
       </c>
@@ -5998,7 +6004,7 @@
       </c>
       <c r="D311"/>
     </row>
-    <row r="312" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>584</v>
       </c>
@@ -6010,7 +6016,7 @@
       </c>
       <c r="D312"/>
     </row>
-    <row r="313" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>586</v>
       </c>
@@ -6022,7 +6028,7 @@
       </c>
       <c r="D313"/>
     </row>
-    <row r="314" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>588</v>
       </c>
@@ -6034,7 +6040,7 @@
       </c>
       <c r="D314"/>
     </row>
-    <row r="315" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>590</v>
       </c>
@@ -6046,7 +6052,7 @@
       </c>
       <c r="D315"/>
     </row>
-    <row r="316" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>592</v>
       </c>
@@ -6058,7 +6064,7 @@
       </c>
       <c r="D316"/>
     </row>
-    <row r="317" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>594</v>
       </c>
@@ -6070,7 +6076,7 @@
       </c>
       <c r="D317"/>
     </row>
-    <row r="318" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>596</v>
       </c>
@@ -6082,7 +6088,7 @@
       </c>
       <c r="D318"/>
     </row>
-    <row r="319" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>598</v>
       </c>
@@ -6094,7 +6100,7 @@
       </c>
       <c r="D319"/>
     </row>
-    <row r="320" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>600</v>
       </c>
@@ -6106,7 +6112,7 @@
       </c>
       <c r="D320"/>
     </row>
-    <row r="321" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>600</v>
       </c>
@@ -6118,7 +6124,7 @@
       </c>
       <c r="D321"/>
     </row>
-    <row r="322" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>600</v>
       </c>
@@ -6130,7 +6136,7 @@
       </c>
       <c r="D322"/>
     </row>
-    <row r="323" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>600</v>
       </c>
@@ -6142,7 +6148,7 @@
       </c>
       <c r="D323"/>
     </row>
-    <row r="324" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>600</v>
       </c>
@@ -6154,7 +6160,7 @@
       </c>
       <c r="D324"/>
     </row>
-    <row r="325" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>606</v>
       </c>
@@ -6166,7 +6172,7 @@
       </c>
       <c r="D325"/>
     </row>
-    <row r="326" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>608</v>
       </c>
@@ -6178,7 +6184,7 @@
       </c>
       <c r="D326"/>
     </row>
-    <row r="327" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>610</v>
       </c>
@@ -6190,7 +6196,7 @@
       </c>
       <c r="D327"/>
     </row>
-    <row r="328" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>612</v>
       </c>
@@ -6202,7 +6208,7 @@
       </c>
       <c r="D328"/>
     </row>
-    <row r="329" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>614</v>
       </c>
@@ -6214,7 +6220,7 @@
       </c>
       <c r="D329"/>
     </row>
-    <row r="330" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>616</v>
       </c>
@@ -6226,7 +6232,7 @@
       </c>
       <c r="D330"/>
     </row>
-    <row r="331" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>618</v>
       </c>
@@ -6255,7 +6261,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>